<commit_message>
Add new examples and modified some old ones
</commit_message>
<xml_diff>
--- a/Examples list for Roman Pilyugin.xlsx
+++ b/Examples list for Roman Pilyugin.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RUpilyuR\Documents\Community review examples projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RUpilyuR\Dropbox\Community review examples projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,6 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <calcPr calcId="171027" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="329">
   <si>
     <t>https://decibel.ni.com/content/docs/DOC-4832</t>
   </si>
@@ -1009,13 +1008,19 @@
   </si>
   <si>
     <t>obsolent toolkit</t>
+  </si>
+  <si>
+    <t>Obsolent toolkit for database access</t>
+  </si>
+  <si>
+    <t>Polymorfic VI. There is no place to put a free label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1033,13 +1038,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1092,12 +1090,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1136,6 +1133,7 @@
       <sheetName val="Stephan Daunke"/>
       <sheetName val="Christoph Deleye"/>
       <sheetName val="Mounzer Saleh"/>
+      <sheetName val="Roman Pilyugin"/>
       <sheetName val="Samah Chazbeck"/>
       <sheetName val="Luis Calderon"/>
       <sheetName val="Xilu Yi"/>
@@ -1146,19 +1144,20 @@
       <sheetName val="Dropdowns"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1463,9 +1462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L292"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,476 +1477,482 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="I2" s="6" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="I7" s="10" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="I7" s="9" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="I10" s="7" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="I10" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="I13" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="I14" s="7" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="6" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="11" t="s">
+    <row r="15" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="J15" s="10" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="J15" s="9" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="I19" s="6" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="I20" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="I21" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="I22" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="I23" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="I23" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="I24" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="I24" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="I25" t="s">
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="I25" s="9" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="J25" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="I26" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="J27" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1955,7 +1960,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1963,7 +1968,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -3876,7 +3881,7 @@
       <c r="A264" t="s">
         <v>1</v>
       </c>
-      <c r="B264" s="6" t="s">
+      <c r="B264" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4120,9 +4125,11 @@
     <hyperlink ref="B15" r:id="rId12"/>
     <hyperlink ref="B16" r:id="rId13"/>
     <hyperlink ref="B18" r:id="rId14"/>
+    <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B25" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>